<commit_message>
ajout nombre dheures consacrees 22jan
</commit_message>
<xml_diff>
--- a/doc/RegistreHeuresConsacrees.xlsx
+++ b/doc/RegistreHeuresConsacrees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\TP3_AMOC_KCarufel_JAudet\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\TP3_AMOC_KCarufel_JAudet\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C2BE91-D9A2-4B0C-9DAD-4975496356C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38312BF-6A60-45C0-A279-10F752F8E218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">Nom </t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Temps consacré (Heure)</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -183,13 +186,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,150 +474,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:J19"/>
+  <dimension ref="C5:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J20" sqref="J20:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="4" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="9">
+        <v>44946</v>
+      </c>
+      <c r="F7" s="5">
         <v>2.5</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="8"/>
+      <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="6" t="s">
+    <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>44948</v>
+      </c>
+      <c r="F8" s="10">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+      <c r="J8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>